<commit_message>
created new script for nonlinear models; changed year to 1-27 in models instead of 1992-2018; created new variable for fish+sponge richness; separated combined models into combined richness predicted by cover and rugosity and fish+sponge richness predicted by coral richness; graphed frequency distributions of response variables
</commit_message>
<xml_diff>
--- a/Results/combined_aic_table.xlsx
+++ b/Results/combined_aic_table.xlsx
@@ -1042,10 +1042,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2502,5 +2505,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="69" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>